<commit_message>
Se añadio en el i -- en el while de la funcion rangos ya que tenia ese bug
</commit_message>
<xml_diff>
--- a/entrada.xlsx
+++ b/entrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanlino/Documents/Semestre7/IA/LogicaDifusa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78861EAA-8B9C-D94B-9EC1-D76DF8ADECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C1DAD2-DC8D-A448-AF5C-404A988E6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,7 +373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -431,7 +433,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>12</v>
+        <v>9.89</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>